<commit_message>
data example for type 2 edited so it matches data in type 1
</commit_message>
<xml_diff>
--- a/template/Example_input/type_2_data.xlsx
+++ b/template/Example_input/type_2_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\11-1-1\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\template\Example_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F58476-B6E2-4DBA-9B44-70B7137589E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9790FA3-6675-4F9B-87E3-D0F90CAC4382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="915" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11532" yWindow="-2622" windowWidth="12168" windowHeight="10752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2008" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>all households</t>
   </si>
@@ -107,10 +107,19 @@
     <t>Source: some source</t>
   </si>
   <si>
-    <t>Example table, 2008</t>
-  </si>
-  <si>
     <t>Example table, 2009</t>
+  </si>
+  <si>
+    <t>Example table, UK, 2008</t>
+  </si>
+  <si>
+    <t>&lt; 66</t>
+  </si>
+  <si>
+    <t>&gt; 65</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -761,38 +770,38 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1160,7 +1169,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="D4" sqref="D4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1185,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1189,7 +1198,7 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
+      <c r="A2" s="42"/>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1201,7 +1210,7 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:20" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6"/>
@@ -1220,12 +1229,12 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="D4" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
@@ -1257,7 +1266,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1271,11 +1280,11 @@
       <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="51" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C7" s="24">
         <v>35.687432872156251</v>
@@ -1308,9 +1317,9 @@
       <c r="R7" s="41"/>
     </row>
     <row r="8" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="23" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C8" s="24">
         <v>33.517168714042498</v>
@@ -1344,7 +1353,7 @@
       <c r="R8" s="41"/>
     </row>
     <row r="9" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="10"/>
       <c r="C9" s="24">
         <v>33.58547418448957</v>
@@ -1378,7 +1387,7 @@
       <c r="R9" s="41"/>
     </row>
     <row r="10" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="51" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -1416,7 +1425,7 @@
       <c r="R10" s="41"/>
     </row>
     <row r="11" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
@@ -1452,7 +1461,7 @@
       <c r="R11" s="41"/>
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="22"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -1472,7 +1481,7 @@
       <c r="R12" s="41"/>
     </row>
     <row r="13" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="32"/>
@@ -1508,21 +1517,21 @@
       <c r="R13" s="41"/>
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
     </row>
     <row r="15" spans="1:20" s="36" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="39"/>
@@ -1545,7 +1554,7 @@
       <c r="T15" s="38"/>
     </row>
     <row r="16" spans="1:20" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="40"/>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
@@ -1567,7 +1576,7 @@
       <c r="T16" s="38"/>
     </row>
     <row r="17" spans="1:20" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="41"/>
       <c r="C17" s="41"/>
       <c r="D17" s="41"/>
@@ -1611,7 +1620,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="47" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="45" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="41" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="9.140625" style="41"/>
     <col min="8" max="8" width="1.7109375" style="41" customWidth="1"/>
@@ -1622,7 +1631,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="41" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1635,7 +1644,7 @@
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
+      <c r="A2" s="42"/>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1647,7 +1656,7 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6"/>
@@ -1666,12 +1675,12 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
@@ -1703,7 +1712,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" s="21" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1717,7 +1726,7 @@
       <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:21" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="51" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="23" t="s">
@@ -1747,7 +1756,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="23" t="s">
         <v>6</v>
       </c>
@@ -1775,7 +1784,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="10"/>
       <c r="C9" s="24">
         <v>26.868379347591659</v>
@@ -1801,7 +1810,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="51" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -1831,7 +1840,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
@@ -1859,7 +1868,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="22"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -1871,7 +1880,7 @@
       <c r="J12" s="31"/>
     </row>
     <row r="13" spans="1:21" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="32"/>
@@ -1899,18 +1908,18 @@
       </c>
     </row>
     <row r="14" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
       <c r="M14" s="37"/>
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
@@ -1922,7 +1931,7 @@
       <c r="U14" s="38"/>
     </row>
     <row r="15" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="39"/>
@@ -1939,7 +1948,7 @@
       <c r="U15" s="38"/>
     </row>
     <row r="16" spans="1:21" s="41" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="40"/>
       <c r="K16" s="38"/>
       <c r="L16" s="38"/>

</xml_diff>